<commit_message>
Fixed projection code for counterfactual scenario (starting in 1984)
</commit_message>
<xml_diff>
--- a/ProjectionControlScenario1.xlsx
+++ b/ProjectionControlScenario1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\V-Notching Study\90historical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mackenzie\Desktop\IBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A500B594-1D2D-446F-BBFC-B7E31A2673BC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D239581-C4B0-42CB-A728-69432B511576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YearToApplyAdaptiveManagement" sheetId="24" r:id="rId1"/>
@@ -31,13 +31,14 @@
     <sheet name="TACProject" sheetId="23" r:id="rId16"/>
     <sheet name="HandlingMProject" sheetId="10" r:id="rId17"/>
     <sheet name="FisheryProbProject" sheetId="12" r:id="rId18"/>
+    <sheet name="VNotchProject" sheetId="25" r:id="rId19"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="240">
   <si>
     <t>Parameters</t>
   </si>
@@ -755,6 +756,9 @@
   <si>
     <t>FisheryProb_30</t>
   </si>
+  <si>
+    <t>V-Notch ratio</t>
+  </si>
 </sst>
 </file>
 
@@ -34664,7 +34668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AH281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -84183,6 +84187,37 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D60BD3-F85D-4379-99A3-BBD48922A341}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H10"/>
@@ -84565,7 +84600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -84588,7 +84623,7 @@
         <v>99</v>
       </c>
       <c r="B2" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -89630,7 +89665,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added input option for recruitment in projections
</commit_message>
<xml_diff>
--- a/ProjectionControlScenario1.xlsx
+++ b/ProjectionControlScenario1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mackenzie\Desktop\IBLS_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EBC62E-95B1-4A0B-AA43-86826B2A2DA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD01CECA-2AAD-42CF-B6D9-F179D4F6AC30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -757,7 +757,7 @@
     <t>V-Notch ratio</t>
   </si>
   <si>
-    <t>recruitment type.  0: random draw from historical recruitment; 1:Ricker; 2: GAM with temperature; 3: "Weak" stock-recruitment relationship (Mazur et al. 2019)</t>
+    <t>recruitment type.  0: random draw from historical recruitment; 1: Input, 2: Ricker; 3: GAM with temperature; 4: "Weak" stock-recruitment relationship (Mazur et al. 2019)</t>
   </si>
 </sst>
 </file>
@@ -84601,7 +84601,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -84623,7 +84623,7 @@
         <v>239</v>
       </c>
       <c r="B2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -84637,7 +84637,7 @@
   <dimension ref="A1:F265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>